<commit_message>
Rebuilt Jacis pathfinder and generated red11
</commit_message>
<xml_diff>
--- a/JacisPathfinder/Debug/Paths.xlsx
+++ b/JacisPathfinder/Debug/Paths.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Paths (version 1)" sheetId="1" r:id="rId1"/>
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1045,14 +1045,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1197,42 +1200,51 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1">
         <v>4</v>
       </c>
-      <c r="D5">
-        <v>16</v>
-      </c>
-      <c r="E5">
+      <c r="D5" s="1">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1">
         <v>280.25</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
         <v>80</v>
       </c>
-      <c r="H5">
-        <v>234</v>
-      </c>
-      <c r="I5">
-        <v>25</v>
-      </c>
-      <c r="J5">
-        <v>118</v>
-      </c>
-      <c r="K5">
-        <v>234</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
+      <c r="H5" s="1">
+        <v>290.25</v>
+      </c>
+      <c r="I5" s="1">
+        <v>75</v>
+      </c>
+      <c r="J5" s="1">
+        <v>120</v>
+      </c>
+      <c r="K5" s="1">
+        <v>290.25</v>
+      </c>
+      <c r="L5" s="1">
+        <v>-30</v>
+      </c>
+      <c r="M5" s="1">
+        <v>140</v>
+      </c>
+      <c r="N5" s="1">
+        <v>255</v>
+      </c>
+      <c r="O5" s="1">
+        <v>-110</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1240,10 +1252,10 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <v>16</v>
@@ -1255,22 +1267,22 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>168</v>
+        <v>80</v>
       </c>
       <c r="H6">
-        <v>210.75</v>
+        <v>234</v>
       </c>
       <c r="I6">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="J6">
-        <v>168</v>
+        <v>118</v>
       </c>
       <c r="K6">
-        <v>222.75</v>
+        <v>234</v>
       </c>
       <c r="L6">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1826,79 +1838,79 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>3</v>
       </c>
-      <c r="D18">
-        <v>16</v>
-      </c>
-      <c r="E18">
+      <c r="D18" s="1">
+        <v>16</v>
+      </c>
+      <c r="E18" s="1">
         <v>160.25</v>
       </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
         <v>112</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="1">
         <v>234</v>
       </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+      <c r="J18" s="1">
         <v>118</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="1">
         <v>234</v>
       </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="L18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>3</v>
       </c>
-      <c r="D19">
-        <v>16</v>
-      </c>
-      <c r="E19">
+      <c r="D19" s="1">
+        <v>16</v>
+      </c>
+      <c r="E19" s="1">
         <v>160.25</v>
       </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
         <v>112</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="1">
         <v>95</v>
       </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
+      <c r="J19" s="1">
         <v>118</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="1">
         <v>95</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2541,6 +2553,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:R32">
+    <sortCondition ref="A2:A32"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>